<commit_message>
ajustes nos algoritmos Dfs Bfs e Bcu para retornarem a distancia
</commit_message>
<xml_diff>
--- a/Algoritmos/Relatório.xlsx
+++ b/Algoritmos/Relatório.xlsx
@@ -479,27 +479,27 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
         <v>19</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[19]</t>
+          <t>[10, 14, 18, 19]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>390</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="H2" t="n">
-        <v>0.000213623046875</v>
+        <v>0.0002052783966064453</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -512,27 +512,27 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[6, 9, 13]</t>
+          <t>[25, 3, 6, 9, 13, 17, 20, 24]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1153</v>
       </c>
       <c r="F3" t="n">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G3" t="n">
-        <v>1.363636363636364</v>
+        <v>1.096774193548387</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0001287460327148438</v>
+        <v>9.226799011230469e-05</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -545,27 +545,27 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C4" t="n">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[17, 20, 31]</t>
+          <t>[31, 38, 39, 40]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>204</v>
       </c>
       <c r="F4" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="G4" t="n">
-        <v>1.583333333333333</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0001022815704345703</v>
+        <v>0.0001003742218017578</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -578,27 +578,27 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="C5" t="n">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[14]</t>
+          <t>[41, 38, 31, 30, 29]</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>355</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="H5" t="n">
-        <v>7.867813110351562e-05</v>
+        <v>0.0001046657562255859</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -611,27 +611,27 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[3, 2, 5, 8, 12]</t>
+          <t>[14, 15, 16, 17, 30]</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>401</v>
       </c>
       <c r="F6" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G6" t="n">
-        <v>1.133333333333333</v>
+        <v>1.3</v>
       </c>
       <c r="H6" t="n">
-        <v>8.821487426757812e-05</v>
+        <v>0.0001049041748046875</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -710,27 +710,27 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
         <v>19</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[19]</t>
+          <t>[10, 14, 15, 16, 19]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>380</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>3121139</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.9999996796041445</v>
       </c>
       <c r="H2" t="n">
-        <v>8.20159912109375e-05</v>
+        <v>1.29628849029541</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -743,27 +743,27 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[6, 3, 2, 5, 4, 7, 8, 9, 28, 29, 13]</t>
+          <t>[25, 26, 27, 28, 29, 30, 31, 32, 24]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>615</v>
       </c>
       <c r="F3" t="n">
-        <v>15</v>
+        <v>2716923</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1333333333333333</v>
+        <v>0.9999996319365694</v>
       </c>
       <c r="H3" t="n">
-        <v>7.796287536621094e-05</v>
+        <v>1.133981943130493</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -776,27 +776,27 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C4" t="n">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[17, 13, 9, 6, 3, 2, 5, 4, 7, 8, 12, 11, 10, 14, 15, 16, 19, 18, 21, 22, 23, 24, 20, 31]</t>
+          <t>[31, 38, 39, 40]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>204</v>
       </c>
       <c r="F4" t="n">
-        <v>25</v>
+        <v>6634523</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.9999998492732635</v>
       </c>
       <c r="H4" t="n">
-        <v>8.344650268554688e-05</v>
+        <v>2.81198787689209</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -809,27 +809,27 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="C5" t="n">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[14]</t>
+          <t>[41, 38, 37, 30, 29]</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>352</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>3349902</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.9999997014838046</v>
       </c>
       <c r="H5" t="n">
-        <v>7.128715515136719e-05</v>
+        <v>1.245441436767578</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -842,27 +842,27 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[3, 2, 5, 4, 7, 8, 9, 6, 27, 28, 29, 13, 12]</t>
+          <t>[14, 15, 16, 17, 30]</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>401</v>
       </c>
       <c r="F6" t="n">
-        <v>16</v>
+        <v>2153983</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0625</v>
+        <v>0.9999995357437825</v>
       </c>
       <c r="H6" t="n">
-        <v>7.414817810058594e-05</v>
+        <v>0.8786857128143311</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -941,27 +941,27 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
         <v>19</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[19]</t>
+          <t>[10, 14, 15, 16, 19]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>380</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.6190476190476191</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0001046657562255859</v>
+        <v>0.0001392364501953125</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -974,27 +974,27 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[6, 9, 13]</t>
+          <t>[25, 26, 27, 28, 29, 30, 31, 32, 24]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>615</v>
       </c>
       <c r="F3" t="n">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.7906976744186046</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0002241134643554688</v>
+        <v>0.0001776218414306641</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -1007,27 +1007,27 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C4" t="n">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[17, 30, 31]</t>
+          <t>[31, 38, 39, 40]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>204</v>
       </c>
       <c r="F4" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G4" t="n">
-        <v>0.4</v>
+        <v>0.5909090909090909</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0001020431518554688</v>
+        <v>8.940696716308594e-05</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -1040,27 +1040,27 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="C5" t="n">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[14]</t>
+          <t>[41, 38, 37, 30, 29]</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>352</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.7727272727272727</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0001242160797119141</v>
+        <v>8.845329284667969e-05</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -1073,27 +1073,27 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[3, 6, 5, 8, 12]</t>
+          <t>[14, 15, 16, 17, 30]</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>401</v>
       </c>
       <c r="F6" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G6" t="n">
-        <v>0.7727272727272727</v>
+        <v>0.76</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0001125335693359375</v>
+        <v>0.0001554489135742188</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -1172,27 +1172,27 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
         <v>19</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[19]</t>
+          <t>[10, 14, 15, 16, 19]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>380</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G2" t="n">
-        <v>3.0625</v>
+        <v>3.071428571428572</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0001130104064941406</v>
+        <v>0.0001668930053710938</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -1205,27 +1205,27 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[6, 9, 13]</t>
+          <t>[25, 26, 27, 28, 29, 30, 31, 32, 24]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>164</v>
+        <v>615</v>
       </c>
       <c r="F3" t="n">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="G3" t="n">
-        <v>3.0625</v>
+        <v>3.071428571428572</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0001275539398193359</v>
+        <v>0.0001673698425292969</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -1238,27 +1238,27 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C4" t="n">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[17, 30, 31]</t>
+          <t>[31, 38, 39, 40]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>166</v>
+        <v>204</v>
       </c>
       <c r="F4" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G4" t="n">
-        <v>3.0625</v>
+        <v>3.071428571428572</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0001168251037597656</v>
+        <v>0.0001206398010253906</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -1271,27 +1271,27 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="C5" t="n">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[14]</t>
+          <t>[41, 38, 37, 30, 29]</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>352</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G5" t="n">
-        <v>3.0625</v>
+        <v>3.071428571428572</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0001053810119628906</v>
+        <v>0.0001127719879150391</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -1304,27 +1304,27 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[3, 6, 5, 8, 12]</t>
+          <t>[14, 15, 16, 17, 30]</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>349</v>
+        <v>401</v>
       </c>
       <c r="F6" t="n">
         <v>16</v>
       </c>
       <c r="G6" t="n">
-        <v>3.0625</v>
+        <v>3.071428571428572</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0004928112030029297</v>
+        <v>0.0001287460327148438</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -1403,27 +1403,27 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
         <v>19</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[19]</t>
+          <t>[10, 14, 15, 16, 19]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>380</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G2" t="n">
-        <v>3.0625</v>
+        <v>3.071428571428572</v>
       </c>
       <c r="H2" t="n">
-        <v>0.003904104232788086</v>
+        <v>0.0002303123474121094</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -1436,27 +1436,27 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[6, 9, 13]</t>
+          <t>[25, 26, 27, 28, 29, 30, 31, 32, 24]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>164</v>
+        <v>615</v>
       </c>
       <c r="F3" t="n">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="G3" t="n">
-        <v>3.0625</v>
+        <v>3.071428571428572</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0001533031463623047</v>
+        <v>0.0001883506774902344</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -1469,27 +1469,27 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C4" t="n">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[17, 30, 31]</t>
+          <t>[31, 38, 39, 40]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>166</v>
+        <v>204</v>
       </c>
       <c r="F4" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G4" t="n">
-        <v>3.0625</v>
+        <v>3.071428571428572</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0001726150512695312</v>
+        <v>0.0001289844512939453</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -1502,27 +1502,27 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="C5" t="n">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[14]</t>
+          <t>[41, 38, 37, 30, 29]</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>352</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G5" t="n">
-        <v>3.0625</v>
+        <v>3.071428571428572</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0001351833343505859</v>
+        <v>0.0001378059387207031</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -1535,27 +1535,27 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[3, 6, 5, 8, 12]</t>
+          <t>[14, 15, 16, 17, 30]</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>349</v>
+        <v>401</v>
       </c>
       <c r="F6" t="n">
         <v>16</v>
       </c>
       <c r="G6" t="n">
-        <v>3.0625</v>
+        <v>3.071428571428572</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0001521110534667969</v>
+        <v>0.0001387596130371094</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
testes de tempo por nós e testes comparando algoritmos feitos e planilhas geradas. Faltando somente o DFS que ainda está para ajustes!
</commit_message>
<xml_diff>
--- a/Algoritmos/Relatório.xlsx
+++ b/Algoritmos/Relatório.xlsx
@@ -479,27 +479,27 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C2" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[10, 14, 18, 19]</t>
+          <t>[23, 19, 16, 12, 8]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>390</v>
+        <v>453</v>
       </c>
       <c r="F2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" t="n">
-        <v>1.333333333333333</v>
+        <v>1.3125</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0002052783966064453</v>
+        <v>0.0003414154052734375</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -512,27 +512,27 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="C3" t="n">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[25, 3, 6, 9, 13, 17, 20, 24]</t>
+          <t>[41, 38, 31, 20, 19, 18]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1153</v>
+        <v>596</v>
       </c>
       <c r="F3" t="n">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="G3" t="n">
-        <v>1.096774193548387</v>
+        <v>1.19047619047619</v>
       </c>
       <c r="H3" t="n">
-        <v>9.226799011230469e-05</v>
+        <v>0.0001759529113769531</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -545,27 +545,27 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[31, 38, 39, 40]</t>
+          <t>[32, 31, 38, 39]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>204</v>
+        <v>253</v>
       </c>
       <c r="F4" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G4" t="n">
-        <v>1.333333333333333</v>
+        <v>1.466666666666667</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0001003742218017578</v>
+        <v>0.0001504421234130859</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -578,27 +578,27 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="C5" t="n">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[41, 38, 31, 30, 29]</t>
+          <t>[12, 8, 5, 4]</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>355</v>
+        <v>448</v>
       </c>
       <c r="F5" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" t="n">
-        <v>1.25</v>
+        <v>1.533333333333333</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0001046657562255859</v>
+        <v>0.0001313686370849609</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -611,27 +611,27 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[14, 15, 16, 17, 30]</t>
+          <t>[21, 18, 14, 10, 7, 8, 9, 28, 34]</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>401</v>
+        <v>1036</v>
       </c>
       <c r="F6" t="n">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="G6" t="n">
-        <v>1.3</v>
+        <v>1.051282051282051</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0001049041748046875</v>
+        <v>0.0001745223999023438</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -710,27 +710,27 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C2" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[10, 14, 15, 16, 19]</t>
+          <t>[23, 19, 16, 12, 8]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>380</v>
+        <v>453</v>
       </c>
       <c r="F2" t="n">
-        <v>3121139</v>
+        <v>3835261</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9999996796041445</v>
+        <v>0.9999997392615522</v>
       </c>
       <c r="H2" t="n">
-        <v>1.29628849029541</v>
+        <v>1.71847128868103</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -743,27 +743,27 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="C3" t="n">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[25, 26, 27, 28, 29, 30, 31, 32, 24]</t>
+          <t>[41, 32, 24, 23, 22, 21, 18]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>615</v>
+        <v>571</v>
       </c>
       <c r="F3" t="n">
-        <v>2716923</v>
+        <v>5113534</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9999996319365694</v>
+        <v>0.9999998044405298</v>
       </c>
       <c r="H3" t="n">
-        <v>1.133981943130493</v>
+        <v>2.365155696868896</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -776,27 +776,27 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[31, 38, 39, 40]</t>
+          <t>[32, 41, 38, 39]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>204</v>
+        <v>252</v>
       </c>
       <c r="F4" t="n">
-        <v>6634523</v>
+        <v>5110434</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9999998492732635</v>
+        <v>0.9999998043219029</v>
       </c>
       <c r="H4" t="n">
-        <v>2.81198787689209</v>
+        <v>2.33404803276062</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -809,27 +809,27 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="C5" t="n">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[41, 38, 37, 30, 29]</t>
+          <t>[12, 8, 7, 4]</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>352</v>
+        <v>438</v>
       </c>
       <c r="F5" t="n">
-        <v>3349902</v>
+        <v>3573789</v>
       </c>
       <c r="G5" t="n">
-        <v>0.9999997014838046</v>
+        <v>0.9999997201849353</v>
       </c>
       <c r="H5" t="n">
-        <v>1.245441436767578</v>
+        <v>1.922887086868286</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -842,27 +842,27 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[14, 15, 16, 17, 30]</t>
+          <t>[21, 18, 14, 15, 16, 17, 30, 29, 28, 34]</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>401</v>
+        <v>706</v>
       </c>
       <c r="F6" t="n">
-        <v>2153983</v>
+        <v>16513894</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9999995357437825</v>
+        <v>0.9999999394449305</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8786857128143311</v>
+        <v>4.870802879333496</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -941,27 +941,27 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C2" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[10, 14, 15, 16, 19]</t>
+          <t>[23, 19, 16, 12, 8]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>380</v>
+        <v>453</v>
       </c>
       <c r="F2" t="n">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6190476190476191</v>
+        <v>0.7352941176470589</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0001392364501953125</v>
+        <v>0.0002031326293945312</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -974,27 +974,27 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="C3" t="n">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[25, 26, 27, 28, 29, 30, 31, 32, 24]</t>
+          <t>[41, 32, 24, 23, 22, 21, 18]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>615</v>
+        <v>571</v>
       </c>
       <c r="F3" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G3" t="n">
-        <v>0.7906976744186046</v>
+        <v>0.8205128205128205</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0001776218414306641</v>
+        <v>0.0002779960632324219</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -1007,27 +1007,27 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[31, 38, 39, 40]</t>
+          <t>[32, 41, 38, 39]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>204</v>
+        <v>252</v>
       </c>
       <c r="F4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5909090909090909</v>
+        <v>0.6</v>
       </c>
       <c r="H4" t="n">
-        <v>8.940696716308594e-05</v>
+        <v>0.0001344680786132812</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -1040,27 +1040,27 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>[12, 8, 7, 4]</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>438</v>
+      </c>
+      <c r="F5" t="n">
         <v>29</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>[41, 38, 37, 30, 29]</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>352</v>
-      </c>
-      <c r="F5" t="n">
-        <v>18</v>
-      </c>
       <c r="G5" t="n">
-        <v>0.7727272727272727</v>
+        <v>0.7</v>
       </c>
       <c r="H5" t="n">
-        <v>8.845329284667969e-05</v>
+        <v>0.0001776218414306641</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -1073,27 +1073,27 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[14, 15, 16, 17, 30]</t>
+          <t>[21, 18, 14, 15, 16, 17, 30, 29, 28, 34]</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>401</v>
+        <v>706</v>
       </c>
       <c r="F6" t="n">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="G6" t="n">
-        <v>0.76</v>
+        <v>0.8461538461538461</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0001554489135742188</v>
+        <v>0.0001685619354248047</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -1172,27 +1172,27 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C2" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[10, 14, 15, 16, 19]</t>
+          <t>[23, 19, 16, 12, 8]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>380</v>
+        <v>453</v>
       </c>
       <c r="F2" t="n">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G2" t="n">
         <v>3.071428571428572</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0001668930053710938</v>
+        <v>0.0002729892730712891</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -1205,27 +1205,27 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="C3" t="n">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[25, 26, 27, 28, 29, 30, 31, 32, 24]</t>
+          <t>[41, 32, 24, 23, 22, 21, 18]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>615</v>
+        <v>571</v>
       </c>
       <c r="F3" t="n">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G3" t="n">
         <v>3.071428571428572</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0001673698425292969</v>
+        <v>0.0002608299255371094</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -1238,27 +1238,27 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[31, 38, 39, 40]</t>
+          <t>[32, 41, 38, 39]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>204</v>
+        <v>252</v>
       </c>
       <c r="F4" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" t="n">
         <v>3.071428571428572</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0001206398010253906</v>
+        <v>0.0001816749572753906</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -1271,27 +1271,27 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="C5" t="n">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[41, 38, 37, 30, 29]</t>
+          <t>[12, 8, 7, 4]</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>352</v>
+        <v>438</v>
       </c>
       <c r="F5" t="n">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="G5" t="n">
         <v>3.071428571428572</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0001127719879150391</v>
+        <v>0.0002675056457519531</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -1304,27 +1304,27 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[14, 15, 16, 17, 30]</t>
+          <t>[21, 18, 14, 15, 16, 17, 30, 29, 28, 34]</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>401</v>
+        <v>706</v>
       </c>
       <c r="F6" t="n">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="G6" t="n">
         <v>3.071428571428572</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0001287460327148438</v>
+        <v>0.0002770423889160156</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -1403,27 +1403,27 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C2" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[10, 14, 15, 16, 19]</t>
+          <t>[23, 19, 16, 12, 8]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>380</v>
+        <v>453</v>
       </c>
       <c r="F2" t="n">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G2" t="n">
         <v>3.071428571428572</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0002303123474121094</v>
+        <v>0.0003378391265869141</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -1436,27 +1436,27 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="C3" t="n">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[25, 26, 27, 28, 29, 30, 31, 32, 24]</t>
+          <t>[41, 32, 24, 23, 22, 21, 18]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>615</v>
+        <v>571</v>
       </c>
       <c r="F3" t="n">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G3" t="n">
         <v>3.071428571428572</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0001883506774902344</v>
+        <v>0.0003247261047363281</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -1469,27 +1469,27 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[31, 38, 39, 40]</t>
+          <t>[32, 41, 38, 39]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>204</v>
+        <v>252</v>
       </c>
       <c r="F4" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" t="n">
         <v>3.071428571428572</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0001289844512939453</v>
+        <v>0.0002036094665527344</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -1502,27 +1502,27 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="C5" t="n">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[41, 38, 37, 30, 29]</t>
+          <t>[12, 8, 7, 4]</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>352</v>
+        <v>438</v>
       </c>
       <c r="F5" t="n">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="G5" t="n">
         <v>3.071428571428572</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0001378059387207031</v>
+        <v>0.00031280517578125</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -1535,27 +1535,27 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[14, 15, 16, 17, 30]</t>
+          <t>[21, 18, 14, 15, 16, 17, 30, 29, 28, 34]</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>401</v>
+        <v>706</v>
       </c>
       <c r="F6" t="n">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="G6" t="n">
         <v>3.071428571428572</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0001387596130371094</v>
+        <v>0.0003390312194824219</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>

</xml_diff>